<commit_message>
Subi los documentos corregidos para el dia 24 de septiembre
</commit_message>
<xml_diff>
--- a/assets/docs/BitacoraTiempo_Desarrollo.xlsx
+++ b/assets/docs/BitacoraTiempo_Desarrollo.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>UNIVERSIDAD PILOTO DE COLOMBIA</t>
   </si>
@@ -150,6 +150,27 @@
   <si>
     <t>Se realizaron las plantillas de la etapa de planificación</t>
   </si>
+  <si>
+    <t>Log de defectos, plan de calidad, script planeación</t>
+  </si>
+  <si>
+    <t>Se realizó el primer log de defectos junto con el arreglo de plan de calidad</t>
+  </si>
+  <si>
+    <t>SDS</t>
+  </si>
+  <si>
+    <t>Se realizó la plantilla de SDS</t>
+  </si>
+  <si>
+    <t>Diagramas</t>
+  </si>
+  <si>
+    <t>Diagrama de información y funcionalidad</t>
+  </si>
+  <si>
+    <t>Diagrama de despliegue, desarrollo, concurrencia, operacional y script</t>
+  </si>
 </sst>
 </file>
 
@@ -235,33 +256,33 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,9 +500,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="57.63"/>
-    <col customWidth="1" min="3" max="3" width="18.75"/>
-    <col customWidth="1" min="4" max="4" width="5.13"/>
+    <col customWidth="1" min="2" max="2" width="13.88"/>
+    <col customWidth="1" min="3" max="3" width="14.5"/>
+    <col customWidth="1" min="4" max="4" width="11.5"/>
     <col customWidth="1" min="5" max="5" width="15.75"/>
     <col customWidth="1" min="6" max="6" width="10.88"/>
     <col customWidth="1" min="7" max="7" width="17.63"/>
@@ -1145,7 +1166,7 @@
         <v>26</v>
       </c>
       <c r="K16" s="6">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -1166,16 +1187,36 @@
     </row>
     <row r="17">
       <c r="A17" s="2"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
+      <c r="B17" s="9">
+        <v>45913.0</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0.54375</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0.5645833333333333</v>
+      </c>
+      <c r="E17" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="F17" s="6">
+        <v>28.0</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" s="6">
+        <v>2.0</v>
+      </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1195,16 +1236,37 @@
     </row>
     <row r="18">
       <c r="A18" s="2"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
+      <c r="B18" s="9">
+        <v>45916.0</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0.9486111111111111</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0.9611111111111111</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F18" s="11">
+        <f>64-46</f>
+        <v>18</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="6">
+        <v>1.0</v>
+      </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1224,16 +1286,36 @@
     </row>
     <row r="19">
       <c r="A19" s="2"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
+      <c r="B19" s="9">
+        <v>45916.0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0.9611111111111111</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0.022916666666666665</v>
+      </c>
+      <c r="E19" s="6">
+        <v>15.0</v>
+      </c>
+      <c r="F19" s="6">
+        <v>74.0</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" s="6">
+        <v>2.0</v>
+      </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1253,16 +1335,36 @@
     </row>
     <row r="20">
       <c r="A20" s="2"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
+      <c r="B20" s="9">
+        <v>45917.0</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0.022916666666666665</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0.05625</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F20" s="6">
+        <v>48.0</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="6">
+        <v>5.0</v>
+      </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>

</xml_diff>